<commit_message>
Added history starting from 2009-March-31 historical data to all stocks
</commit_message>
<xml_diff>
--- a/data/0178.xlsx
+++ b/data/0178.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1145"/>
+  <dimension ref="A1:I1154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37988,11 +37988,11 @@
     </row>
     <row r="1073">
       <c r="A1073" t="n">
-        <v>1574985600</v>
+        <v>1574035200</v>
       </c>
       <c r="B1073" t="inlineStr">
         <is>
-          <t>2019-11-29</t>
+          <t>2019-11-18</t>
         </is>
       </c>
       <c r="C1073" t="inlineStr">
@@ -38006,28 +38006,28 @@
         </is>
       </c>
       <c r="E1073" t="n">
-        <v>0.17</v>
+        <v>0.165</v>
       </c>
       <c r="F1073" t="n">
-        <v>0.17</v>
+        <v>0.165</v>
       </c>
       <c r="G1073" t="n">
         <v>0.16</v>
       </c>
       <c r="H1073" t="n">
-        <v>0.165</v>
+        <v>0.16</v>
       </c>
       <c r="I1073" t="n">
-        <v>1765100</v>
+        <v>692900</v>
       </c>
     </row>
     <row r="1074">
       <c r="A1074" t="n">
-        <v>1575244800</v>
+        <v>1574121600</v>
       </c>
       <c r="B1074" t="inlineStr">
         <is>
-          <t>2019-12-02</t>
+          <t>2019-11-19</t>
         </is>
       </c>
       <c r="C1074" t="inlineStr">
@@ -38041,28 +38041,28 @@
         </is>
       </c>
       <c r="E1074" t="n">
-        <v>0.165</v>
+        <v>0.16</v>
       </c>
       <c r="F1074" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="G1074" t="n">
-        <v>0.165</v>
+        <v>0.155</v>
       </c>
       <c r="H1074" t="n">
-        <v>0.18</v>
+        <v>0.155</v>
       </c>
       <c r="I1074" t="n">
-        <v>4032500</v>
+        <v>706000</v>
       </c>
     </row>
     <row r="1075">
       <c r="A1075" t="n">
-        <v>1575331200</v>
+        <v>1574208000</v>
       </c>
       <c r="B1075" t="inlineStr">
         <is>
-          <t>2019-12-03</t>
+          <t>2019-11-20</t>
         </is>
       </c>
       <c r="C1075" t="inlineStr">
@@ -38076,28 +38076,28 @@
         </is>
       </c>
       <c r="E1075" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="F1075" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="G1075" t="n">
-        <v>0.175</v>
+        <v>0.15</v>
       </c>
       <c r="H1075" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="I1075" t="n">
-        <v>3216600</v>
+        <v>1784300</v>
       </c>
     </row>
     <row r="1076">
       <c r="A1076" t="n">
-        <v>1575417600</v>
+        <v>1574294400</v>
       </c>
       <c r="B1076" t="inlineStr">
         <is>
-          <t>2019-12-04</t>
+          <t>2019-11-21</t>
         </is>
       </c>
       <c r="C1076" t="inlineStr">
@@ -38111,28 +38111,28 @@
         </is>
       </c>
       <c r="E1076" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="F1076" t="n">
         <v>0.18</v>
       </c>
-      <c r="F1076" t="n">
-        <v>0.185</v>
-      </c>
       <c r="G1076" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H1076" t="n">
         <v>0.175</v>
       </c>
-      <c r="H1076" t="n">
-        <v>0.185</v>
-      </c>
       <c r="I1076" t="n">
-        <v>2328400</v>
+        <v>4138800</v>
       </c>
     </row>
     <row r="1077">
       <c r="A1077" t="n">
-        <v>1575504000</v>
+        <v>1574380800</v>
       </c>
       <c r="B1077" t="inlineStr">
         <is>
-          <t>2019-12-05</t>
+          <t>2019-11-22</t>
         </is>
       </c>
       <c r="C1077" t="inlineStr">
@@ -38146,28 +38146,28 @@
         </is>
       </c>
       <c r="E1077" t="n">
-        <v>0.185</v>
+        <v>0.17</v>
       </c>
       <c r="F1077" t="n">
-        <v>0.2</v>
+        <v>0.175</v>
       </c>
       <c r="G1077" t="n">
-        <v>0.185</v>
+        <v>0.165</v>
       </c>
       <c r="H1077" t="n">
-        <v>0.195</v>
+        <v>0.175</v>
       </c>
       <c r="I1077" t="n">
-        <v>10957000</v>
+        <v>468000</v>
       </c>
     </row>
     <row r="1078">
       <c r="A1078" t="n">
-        <v>1575590400</v>
+        <v>1574640000</v>
       </c>
       <c r="B1078" t="inlineStr">
         <is>
-          <t>2019-12-06</t>
+          <t>2019-11-25</t>
         </is>
       </c>
       <c r="C1078" t="inlineStr">
@@ -38181,28 +38181,28 @@
         </is>
       </c>
       <c r="E1078" t="n">
-        <v>0.2</v>
+        <v>0.175</v>
       </c>
       <c r="F1078" t="n">
-        <v>0.225</v>
+        <v>0.175</v>
       </c>
       <c r="G1078" t="n">
-        <v>0.195</v>
+        <v>0.165</v>
       </c>
       <c r="H1078" t="n">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="I1078" t="n">
-        <v>20264000</v>
+        <v>557300</v>
       </c>
     </row>
     <row r="1079">
       <c r="A1079" t="n">
-        <v>1575849600</v>
+        <v>1574726400</v>
       </c>
       <c r="B1079" t="inlineStr">
         <is>
-          <t>2019-12-09</t>
+          <t>2019-11-26</t>
         </is>
       </c>
       <c r="C1079" t="inlineStr">
@@ -38216,28 +38216,28 @@
         </is>
       </c>
       <c r="E1079" t="n">
-        <v>0.225</v>
+        <v>0.165</v>
       </c>
       <c r="F1079" t="n">
-        <v>0.23</v>
+        <v>0.175</v>
       </c>
       <c r="G1079" t="n">
-        <v>0.215</v>
+        <v>0.165</v>
       </c>
       <c r="H1079" t="n">
-        <v>0.215</v>
+        <v>0.165</v>
       </c>
       <c r="I1079" t="n">
-        <v>11611400</v>
+        <v>1459100</v>
       </c>
     </row>
     <row r="1080">
       <c r="A1080" t="n">
-        <v>1575936000</v>
+        <v>1574812800</v>
       </c>
       <c r="B1080" t="inlineStr">
         <is>
-          <t>2019-12-10</t>
+          <t>2019-11-27</t>
         </is>
       </c>
       <c r="C1080" t="inlineStr">
@@ -38251,28 +38251,28 @@
         </is>
       </c>
       <c r="E1080" t="n">
-        <v>0.215</v>
+        <v>0.16</v>
       </c>
       <c r="F1080" t="n">
-        <v>0.215</v>
+        <v>0.16</v>
       </c>
       <c r="G1080" t="n">
-        <v>0.195</v>
+        <v>0.16</v>
       </c>
       <c r="H1080" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="I1080" t="n">
-        <v>4627900</v>
+        <v>277500</v>
       </c>
     </row>
     <row r="1081">
       <c r="A1081" t="n">
-        <v>1576022400</v>
+        <v>1574899200</v>
       </c>
       <c r="B1081" t="inlineStr">
         <is>
-          <t>2019-12-11</t>
+          <t>2019-11-28</t>
         </is>
       </c>
       <c r="C1081" t="inlineStr">
@@ -38286,28 +38286,28 @@
         </is>
       </c>
       <c r="E1081" t="n">
-        <v>0.2</v>
+        <v>0.155</v>
       </c>
       <c r="F1081" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="G1081" t="n">
-        <v>0.18</v>
+        <v>0.155</v>
       </c>
       <c r="H1081" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="I1081" t="n">
-        <v>6837600</v>
+        <v>264000</v>
       </c>
     </row>
     <row r="1082">
       <c r="A1082" t="n">
-        <v>1576108800</v>
+        <v>1574985600</v>
       </c>
       <c r="B1082" t="inlineStr">
         <is>
-          <t>2019-12-12</t>
+          <t>2019-11-29</t>
         </is>
       </c>
       <c r="C1082" t="inlineStr">
@@ -38321,28 +38321,28 @@
         </is>
       </c>
       <c r="E1082" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F1082" t="n">
-        <v>0.195</v>
+        <v>0.17</v>
       </c>
       <c r="G1082" t="n">
-        <v>0.185</v>
+        <v>0.16</v>
       </c>
       <c r="H1082" t="n">
-        <v>0.19</v>
+        <v>0.165</v>
       </c>
       <c r="I1082" t="n">
-        <v>3797000</v>
+        <v>1765100</v>
       </c>
     </row>
     <row r="1083">
       <c r="A1083" t="n">
-        <v>1576195200</v>
+        <v>1575244800</v>
       </c>
       <c r="B1083" t="inlineStr">
         <is>
-          <t>2019-12-13</t>
+          <t>2019-12-02</t>
         </is>
       </c>
       <c r="C1083" t="inlineStr">
@@ -38356,28 +38356,28 @@
         </is>
       </c>
       <c r="E1083" t="n">
-        <v>0.185</v>
+        <v>0.165</v>
       </c>
       <c r="F1083" t="n">
-        <v>0.195</v>
+        <v>0.19</v>
       </c>
       <c r="G1083" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="H1083" t="n">
         <v>0.18</v>
       </c>
-      <c r="H1083" t="n">
-        <v>0.185</v>
-      </c>
       <c r="I1083" t="n">
-        <v>3176300</v>
+        <v>4032500</v>
       </c>
     </row>
     <row r="1084">
       <c r="A1084" t="n">
-        <v>1576454400</v>
+        <v>1575331200</v>
       </c>
       <c r="B1084" t="inlineStr">
         <is>
-          <t>2019-12-16</t>
+          <t>2019-12-03</t>
         </is>
       </c>
       <c r="C1084" t="inlineStr">
@@ -38391,28 +38391,28 @@
         </is>
       </c>
       <c r="E1084" t="n">
-        <v>0.185</v>
+        <v>0.18</v>
       </c>
       <c r="F1084" t="n">
         <v>0.19</v>
       </c>
       <c r="G1084" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="H1084" t="n">
         <v>0.18</v>
       </c>
-      <c r="H1084" t="n">
-        <v>0.185</v>
-      </c>
       <c r="I1084" t="n">
-        <v>3150400</v>
+        <v>3216600</v>
       </c>
     </row>
     <row r="1085">
       <c r="A1085" t="n">
-        <v>1576540800</v>
+        <v>1575417600</v>
       </c>
       <c r="B1085" t="inlineStr">
         <is>
-          <t>2019-12-17</t>
+          <t>2019-12-04</t>
         </is>
       </c>
       <c r="C1085" t="inlineStr">
@@ -38426,28 +38426,28 @@
         </is>
       </c>
       <c r="E1085" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="F1085" t="n">
         <v>0.185</v>
       </c>
-      <c r="F1085" t="n">
-        <v>0.21</v>
-      </c>
       <c r="G1085" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="H1085" t="n">
         <v>0.185</v>
       </c>
-      <c r="H1085" t="n">
-        <v>0.21</v>
-      </c>
       <c r="I1085" t="n">
-        <v>9218400</v>
+        <v>2328400</v>
       </c>
     </row>
     <row r="1086">
       <c r="A1086" t="n">
-        <v>1576627200</v>
+        <v>1575504000</v>
       </c>
       <c r="B1086" t="inlineStr">
         <is>
-          <t>2019-12-18</t>
+          <t>2019-12-05</t>
         </is>
       </c>
       <c r="C1086" t="inlineStr">
@@ -38461,28 +38461,28 @@
         </is>
       </c>
       <c r="E1086" t="n">
-        <v>0.21</v>
+        <v>0.185</v>
       </c>
       <c r="F1086" t="n">
-        <v>0.215</v>
+        <v>0.2</v>
       </c>
       <c r="G1086" t="n">
-        <v>0.205</v>
+        <v>0.185</v>
       </c>
       <c r="H1086" t="n">
-        <v>0.21</v>
+        <v>0.195</v>
       </c>
       <c r="I1086" t="n">
-        <v>2828600</v>
+        <v>10957000</v>
       </c>
     </row>
     <row r="1087">
       <c r="A1087" t="n">
-        <v>1576713600</v>
+        <v>1575590400</v>
       </c>
       <c r="B1087" t="inlineStr">
         <is>
-          <t>2019-12-19</t>
+          <t>2019-12-06</t>
         </is>
       </c>
       <c r="C1087" t="inlineStr">
@@ -38496,28 +38496,28 @@
         </is>
       </c>
       <c r="E1087" t="n">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="F1087" t="n">
-        <v>0.21</v>
+        <v>0.225</v>
       </c>
       <c r="G1087" t="n">
-        <v>0.19</v>
+        <v>0.195</v>
       </c>
       <c r="H1087" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="I1087" t="n">
-        <v>2896800</v>
+        <v>20264000</v>
       </c>
     </row>
     <row r="1088">
       <c r="A1088" t="n">
-        <v>1576800000</v>
+        <v>1575849600</v>
       </c>
       <c r="B1088" t="inlineStr">
         <is>
-          <t>2019-12-20</t>
+          <t>2019-12-09</t>
         </is>
       </c>
       <c r="C1088" t="inlineStr">
@@ -38531,28 +38531,28 @@
         </is>
       </c>
       <c r="E1088" t="n">
-        <v>0.195</v>
+        <v>0.225</v>
       </c>
       <c r="F1088" t="n">
-        <v>0.205</v>
+        <v>0.23</v>
       </c>
       <c r="G1088" t="n">
-        <v>0.19</v>
+        <v>0.215</v>
       </c>
       <c r="H1088" t="n">
-        <v>0.195</v>
+        <v>0.215</v>
       </c>
       <c r="I1088" t="n">
-        <v>2422700</v>
+        <v>11611400</v>
       </c>
     </row>
     <row r="1089">
       <c r="A1089" t="n">
-        <v>1577059200</v>
+        <v>1575936000</v>
       </c>
       <c r="B1089" t="inlineStr">
         <is>
-          <t>2019-12-23</t>
+          <t>2019-12-10</t>
         </is>
       </c>
       <c r="C1089" t="inlineStr">
@@ -38566,10 +38566,10 @@
         </is>
       </c>
       <c r="E1089" t="n">
-        <v>0.195</v>
+        <v>0.215</v>
       </c>
       <c r="F1089" t="n">
-        <v>0.21</v>
+        <v>0.215</v>
       </c>
       <c r="G1089" t="n">
         <v>0.195</v>
@@ -38578,16 +38578,16 @@
         <v>0.2</v>
       </c>
       <c r="I1089" t="n">
-        <v>2752500</v>
+        <v>4627900</v>
       </c>
     </row>
     <row r="1090">
       <c r="A1090" t="n">
-        <v>1577145600</v>
+        <v>1576022400</v>
       </c>
       <c r="B1090" t="inlineStr">
         <is>
-          <t>2019-12-24</t>
+          <t>2019-12-11</t>
         </is>
       </c>
       <c r="C1090" t="inlineStr">
@@ -38601,28 +38601,28 @@
         </is>
       </c>
       <c r="E1090" t="n">
-        <v>0.205</v>
+        <v>0.2</v>
       </c>
       <c r="F1090" t="n">
-        <v>0.205</v>
+        <v>0.2</v>
       </c>
       <c r="G1090" t="n">
-        <v>0.195</v>
+        <v>0.18</v>
       </c>
       <c r="H1090" t="n">
-        <v>0.205</v>
+        <v>0.19</v>
       </c>
       <c r="I1090" t="n">
-        <v>1602100</v>
+        <v>6837600</v>
       </c>
     </row>
     <row r="1091">
       <c r="A1091" t="n">
-        <v>1577318400</v>
+        <v>1576108800</v>
       </c>
       <c r="B1091" t="inlineStr">
         <is>
-          <t>2019-12-26</t>
+          <t>2019-12-12</t>
         </is>
       </c>
       <c r="C1091" t="inlineStr">
@@ -38636,28 +38636,28 @@
         </is>
       </c>
       <c r="E1091" t="n">
-        <v>0.205</v>
+        <v>0.19</v>
       </c>
       <c r="F1091" t="n">
-        <v>0.215</v>
+        <v>0.195</v>
       </c>
       <c r="G1091" t="n">
-        <v>0.2</v>
+        <v>0.185</v>
       </c>
       <c r="H1091" t="n">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="I1091" t="n">
-        <v>4636400</v>
+        <v>3797000</v>
       </c>
     </row>
     <row r="1092">
       <c r="A1092" t="n">
-        <v>1577404800</v>
+        <v>1576195200</v>
       </c>
       <c r="B1092" t="inlineStr">
         <is>
-          <t>2019-12-27</t>
+          <t>2019-12-13</t>
         </is>
       </c>
       <c r="C1092" t="inlineStr">
@@ -38671,28 +38671,28 @@
         </is>
       </c>
       <c r="E1092" t="n">
-        <v>0.215</v>
+        <v>0.185</v>
       </c>
       <c r="F1092" t="n">
-        <v>0.225</v>
+        <v>0.195</v>
       </c>
       <c r="G1092" t="n">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="H1092" t="n">
-        <v>0.21</v>
+        <v>0.185</v>
       </c>
       <c r="I1092" t="n">
-        <v>5024500</v>
+        <v>3176300</v>
       </c>
     </row>
     <row r="1093">
       <c r="A1093" t="n">
-        <v>1577664000</v>
+        <v>1576454400</v>
       </c>
       <c r="B1093" t="inlineStr">
         <is>
-          <t>2019-12-30</t>
+          <t>2019-12-16</t>
         </is>
       </c>
       <c r="C1093" t="inlineStr">
@@ -38706,28 +38706,28 @@
         </is>
       </c>
       <c r="E1093" t="n">
-        <v>0.21</v>
+        <v>0.185</v>
       </c>
       <c r="F1093" t="n">
-        <v>0.215</v>
+        <v>0.19</v>
       </c>
       <c r="G1093" t="n">
-        <v>0.205</v>
+        <v>0.18</v>
       </c>
       <c r="H1093" t="n">
-        <v>0.21</v>
+        <v>0.185</v>
       </c>
       <c r="I1093" t="n">
-        <v>1947500</v>
+        <v>3150400</v>
       </c>
     </row>
     <row r="1094">
       <c r="A1094" t="n">
-        <v>1577750400</v>
+        <v>1576540800</v>
       </c>
       <c r="B1094" t="inlineStr">
         <is>
-          <t>2019-12-31</t>
+          <t>2019-12-17</t>
         </is>
       </c>
       <c r="C1094" t="inlineStr">
@@ -38741,28 +38741,28 @@
         </is>
       </c>
       <c r="E1094" t="n">
-        <v>0.205</v>
+        <v>0.185</v>
       </c>
       <c r="F1094" t="n">
-        <v>0.205</v>
+        <v>0.21</v>
       </c>
       <c r="G1094" t="n">
-        <v>0.195</v>
+        <v>0.185</v>
       </c>
       <c r="H1094" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="I1094" t="n">
-        <v>2206700</v>
+        <v>9218400</v>
       </c>
     </row>
     <row r="1095">
       <c r="A1095" t="n">
-        <v>1577923200</v>
+        <v>1576627200</v>
       </c>
       <c r="B1095" t="inlineStr">
         <is>
-          <t>2020-01-02</t>
+          <t>2019-12-18</t>
         </is>
       </c>
       <c r="C1095" t="inlineStr">
@@ -38776,28 +38776,28 @@
         </is>
       </c>
       <c r="E1095" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="F1095" t="n">
-        <v>0.225</v>
+        <v>0.215</v>
       </c>
       <c r="G1095" t="n">
-        <v>0.2</v>
+        <v>0.205</v>
       </c>
       <c r="H1095" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="I1095" t="n">
-        <v>5274900</v>
+        <v>2828600</v>
       </c>
     </row>
     <row r="1096">
       <c r="A1096" t="n">
-        <v>1578009600</v>
+        <v>1576713600</v>
       </c>
       <c r="B1096" t="inlineStr">
         <is>
-          <t>2020-01-03</t>
+          <t>2019-12-19</t>
         </is>
       </c>
       <c r="C1096" t="inlineStr">
@@ -38811,28 +38811,28 @@
         </is>
       </c>
       <c r="E1096" t="n">
-        <v>0.225</v>
+        <v>0.21</v>
       </c>
       <c r="F1096" t="n">
-        <v>0.255</v>
+        <v>0.21</v>
       </c>
       <c r="G1096" t="n">
-        <v>0.225</v>
+        <v>0.19</v>
       </c>
       <c r="H1096" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="I1096" t="n">
-        <v>19323500</v>
+        <v>2896800</v>
       </c>
     </row>
     <row r="1097">
       <c r="A1097" t="n">
-        <v>1578268800</v>
+        <v>1576800000</v>
       </c>
       <c r="B1097" t="inlineStr">
         <is>
-          <t>2020-01-06</t>
+          <t>2019-12-20</t>
         </is>
       </c>
       <c r="C1097" t="inlineStr">
@@ -38846,28 +38846,28 @@
         </is>
       </c>
       <c r="E1097" t="n">
-        <v>0.245</v>
+        <v>0.195</v>
       </c>
       <c r="F1097" t="n">
-        <v>0.245</v>
+        <v>0.205</v>
       </c>
       <c r="G1097" t="n">
-        <v>0.225</v>
+        <v>0.19</v>
       </c>
       <c r="H1097" t="n">
-        <v>0.24</v>
+        <v>0.195</v>
       </c>
       <c r="I1097" t="n">
-        <v>4092500</v>
+        <v>2422700</v>
       </c>
     </row>
     <row r="1098">
       <c r="A1098" t="n">
-        <v>1578355200</v>
+        <v>1577059200</v>
       </c>
       <c r="B1098" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
+          <t>2019-12-23</t>
         </is>
       </c>
       <c r="C1098" t="inlineStr">
@@ -38881,28 +38881,28 @@
         </is>
       </c>
       <c r="E1098" t="n">
-        <v>0.24</v>
+        <v>0.195</v>
       </c>
       <c r="F1098" t="n">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="G1098" t="n">
-        <v>0.23</v>
+        <v>0.195</v>
       </c>
       <c r="H1098" t="n">
-        <v>0.245</v>
+        <v>0.2</v>
       </c>
       <c r="I1098" t="n">
-        <v>10735000</v>
+        <v>2752500</v>
       </c>
     </row>
     <row r="1099">
       <c r="A1099" t="n">
-        <v>1578441600</v>
+        <v>1577145600</v>
       </c>
       <c r="B1099" t="inlineStr">
         <is>
-          <t>2020-01-08</t>
+          <t>2019-12-24</t>
         </is>
       </c>
       <c r="C1099" t="inlineStr">
@@ -38916,28 +38916,28 @@
         </is>
       </c>
       <c r="E1099" t="n">
-        <v>0.23</v>
+        <v>0.205</v>
       </c>
       <c r="F1099" t="n">
-        <v>0.24</v>
+        <v>0.205</v>
       </c>
       <c r="G1099" t="n">
-        <v>0.215</v>
+        <v>0.195</v>
       </c>
       <c r="H1099" t="n">
-        <v>0.23</v>
+        <v>0.205</v>
       </c>
       <c r="I1099" t="n">
-        <v>6942700</v>
+        <v>1602100</v>
       </c>
     </row>
     <row r="1100">
       <c r="A1100" t="n">
-        <v>1578528000</v>
+        <v>1577318400</v>
       </c>
       <c r="B1100" t="inlineStr">
         <is>
-          <t>2020-01-09</t>
+          <t>2019-12-26</t>
         </is>
       </c>
       <c r="C1100" t="inlineStr">
@@ -38951,28 +38951,28 @@
         </is>
       </c>
       <c r="E1100" t="n">
-        <v>0.23</v>
+        <v>0.205</v>
       </c>
       <c r="F1100" t="n">
-        <v>0.245</v>
+        <v>0.215</v>
       </c>
       <c r="G1100" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="H1100" t="n">
-        <v>0.235</v>
+        <v>0.21</v>
       </c>
       <c r="I1100" t="n">
-        <v>5755700</v>
+        <v>4636400</v>
       </c>
     </row>
     <row r="1101">
       <c r="A1101" t="n">
-        <v>1578614400</v>
+        <v>1577404800</v>
       </c>
       <c r="B1101" t="inlineStr">
         <is>
-          <t>2020-01-10</t>
+          <t>2019-12-27</t>
         </is>
       </c>
       <c r="C1101" t="inlineStr">
@@ -38986,28 +38986,28 @@
         </is>
       </c>
       <c r="E1101" t="n">
-        <v>0.24</v>
+        <v>0.215</v>
       </c>
       <c r="F1101" t="n">
-        <v>0.27</v>
+        <v>0.225</v>
       </c>
       <c r="G1101" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="H1101" t="n">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="I1101" t="n">
-        <v>10873900</v>
+        <v>5024500</v>
       </c>
     </row>
     <row r="1102">
       <c r="A1102" t="n">
-        <v>1578873600</v>
+        <v>1577664000</v>
       </c>
       <c r="B1102" t="inlineStr">
         <is>
-          <t>2020-01-13</t>
+          <t>2019-12-30</t>
         </is>
       </c>
       <c r="C1102" t="inlineStr">
@@ -39021,28 +39021,28 @@
         </is>
       </c>
       <c r="E1102" t="n">
-        <v>0.255</v>
+        <v>0.21</v>
       </c>
       <c r="F1102" t="n">
-        <v>0.275</v>
+        <v>0.215</v>
       </c>
       <c r="G1102" t="n">
-        <v>0.25</v>
+        <v>0.205</v>
       </c>
       <c r="H1102" t="n">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="I1102" t="n">
-        <v>10089200</v>
+        <v>1947500</v>
       </c>
     </row>
     <row r="1103">
       <c r="A1103" t="n">
-        <v>1578960000</v>
+        <v>1577750400</v>
       </c>
       <c r="B1103" t="inlineStr">
         <is>
-          <t>2020-01-14</t>
+          <t>2019-12-31</t>
         </is>
       </c>
       <c r="C1103" t="inlineStr">
@@ -39056,28 +39056,28 @@
         </is>
       </c>
       <c r="E1103" t="n">
-        <v>0.27</v>
+        <v>0.205</v>
       </c>
       <c r="F1103" t="n">
-        <v>0.275</v>
+        <v>0.205</v>
       </c>
       <c r="G1103" t="n">
-        <v>0.255</v>
+        <v>0.195</v>
       </c>
       <c r="H1103" t="n">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="I1103" t="n">
-        <v>6133400</v>
+        <v>2206700</v>
       </c>
     </row>
     <row r="1104">
       <c r="A1104" t="n">
-        <v>1579046400</v>
+        <v>1577923200</v>
       </c>
       <c r="B1104" t="inlineStr">
         <is>
-          <t>2020-01-15</t>
+          <t>2020-01-02</t>
         </is>
       </c>
       <c r="C1104" t="inlineStr">
@@ -39091,28 +39091,28 @@
         </is>
       </c>
       <c r="E1104" t="n">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="F1104" t="n">
-        <v>0.26</v>
+        <v>0.225</v>
       </c>
       <c r="G1104" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H1104" t="n">
-        <v>0.255</v>
+        <v>0.22</v>
       </c>
       <c r="I1104" t="n">
-        <v>2192000</v>
+        <v>5274900</v>
       </c>
     </row>
     <row r="1105">
       <c r="A1105" t="n">
-        <v>1579132800</v>
+        <v>1578009600</v>
       </c>
       <c r="B1105" t="inlineStr">
         <is>
-          <t>2020-01-16</t>
+          <t>2020-01-03</t>
         </is>
       </c>
       <c r="C1105" t="inlineStr">
@@ -39126,28 +39126,28 @@
         </is>
       </c>
       <c r="E1105" t="n">
-        <v>0.26</v>
+        <v>0.225</v>
       </c>
       <c r="F1105" t="n">
-        <v>0.265</v>
+        <v>0.255</v>
       </c>
       <c r="G1105" t="n">
-        <v>0.25</v>
+        <v>0.225</v>
       </c>
       <c r="H1105" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="I1105" t="n">
-        <v>7498700</v>
+        <v>19323500</v>
       </c>
     </row>
     <row r="1106">
       <c r="A1106" t="n">
-        <v>1579219200</v>
+        <v>1578268800</v>
       </c>
       <c r="B1106" t="inlineStr">
         <is>
-          <t>2020-01-17</t>
+          <t>2020-01-06</t>
         </is>
       </c>
       <c r="C1106" t="inlineStr">
@@ -39161,28 +39161,28 @@
         </is>
       </c>
       <c r="E1106" t="n">
-        <v>0.25</v>
+        <v>0.245</v>
       </c>
       <c r="F1106" t="n">
-        <v>0.25</v>
+        <v>0.245</v>
       </c>
       <c r="G1106" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="H1106" t="n">
         <v>0.24</v>
       </c>
-      <c r="H1106" t="n">
-        <v>0.245</v>
-      </c>
       <c r="I1106" t="n">
-        <v>2703700</v>
+        <v>4092500</v>
       </c>
     </row>
     <row r="1107">
       <c r="A1107" t="n">
-        <v>1579478400</v>
+        <v>1578355200</v>
       </c>
       <c r="B1107" t="inlineStr">
         <is>
-          <t>2020-01-20</t>
+          <t>2020-01-07</t>
         </is>
       </c>
       <c r="C1107" t="inlineStr">
@@ -39196,28 +39196,28 @@
         </is>
       </c>
       <c r="E1107" t="n">
-        <v>0.245</v>
+        <v>0.24</v>
       </c>
       <c r="F1107" t="n">
         <v>0.26</v>
       </c>
       <c r="G1107" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="H1107" t="n">
-        <v>0.255</v>
+        <v>0.245</v>
       </c>
       <c r="I1107" t="n">
-        <v>4433500</v>
+        <v>10735000</v>
       </c>
     </row>
     <row r="1108">
       <c r="A1108" t="n">
-        <v>1579564800</v>
+        <v>1578441600</v>
       </c>
       <c r="B1108" t="inlineStr">
         <is>
-          <t>2020-01-21</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="C1108" t="inlineStr">
@@ -39231,28 +39231,28 @@
         </is>
       </c>
       <c r="E1108" t="n">
-        <v>0.26</v>
+        <v>0.23</v>
       </c>
       <c r="F1108" t="n">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="G1108" t="n">
-        <v>0.24</v>
+        <v>0.215</v>
       </c>
       <c r="H1108" t="n">
-        <v>0.245</v>
+        <v>0.23</v>
       </c>
       <c r="I1108" t="n">
-        <v>3318600</v>
+        <v>6942700</v>
       </c>
     </row>
     <row r="1109">
       <c r="A1109" t="n">
-        <v>1579651200</v>
+        <v>1578528000</v>
       </c>
       <c r="B1109" t="inlineStr">
         <is>
-          <t>2020-01-22</t>
+          <t>2020-01-09</t>
         </is>
       </c>
       <c r="C1109" t="inlineStr">
@@ -39266,28 +39266,28 @@
         </is>
       </c>
       <c r="E1109" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F1109" t="n">
         <v>0.245</v>
       </c>
       <c r="G1109" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="H1109" t="n">
-        <v>0.24</v>
+        <v>0.235</v>
       </c>
       <c r="I1109" t="n">
-        <v>2870300</v>
+        <v>5755700</v>
       </c>
     </row>
     <row r="1110">
       <c r="A1110" t="n">
-        <v>1579737600</v>
+        <v>1578614400</v>
       </c>
       <c r="B1110" t="inlineStr">
         <is>
-          <t>2020-01-23</t>
+          <t>2020-01-10</t>
         </is>
       </c>
       <c r="C1110" t="inlineStr">
@@ -39304,25 +39304,25 @@
         <v>0.24</v>
       </c>
       <c r="F1110" t="n">
-        <v>0.255</v>
+        <v>0.27</v>
       </c>
       <c r="G1110" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="H1110" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="I1110" t="n">
-        <v>5798100</v>
+        <v>10873900</v>
       </c>
     </row>
     <row r="1111">
       <c r="A1111" t="n">
-        <v>1579824000</v>
+        <v>1578873600</v>
       </c>
       <c r="B1111" t="inlineStr">
         <is>
-          <t>2020-01-24</t>
+          <t>2020-01-13</t>
         </is>
       </c>
       <c r="C1111" t="inlineStr">
@@ -39336,28 +39336,28 @@
         </is>
       </c>
       <c r="E1111" t="n">
-        <v>0.235</v>
+        <v>0.255</v>
       </c>
       <c r="F1111" t="n">
-        <v>0.245</v>
+        <v>0.275</v>
       </c>
       <c r="G1111" t="n">
-        <v>0.235</v>
+        <v>0.25</v>
       </c>
       <c r="H1111" t="n">
-        <v>0.245</v>
+        <v>0.27</v>
       </c>
       <c r="I1111" t="n">
-        <v>1280400</v>
+        <v>10089200</v>
       </c>
     </row>
     <row r="1112">
       <c r="A1112" t="n">
-        <v>1580169600</v>
+        <v>1578960000</v>
       </c>
       <c r="B1112" t="inlineStr">
         <is>
-          <t>2020-01-28</t>
+          <t>2020-01-14</t>
         </is>
       </c>
       <c r="C1112" t="inlineStr">
@@ -39371,28 +39371,28 @@
         </is>
       </c>
       <c r="E1112" t="n">
-        <v>0.235</v>
+        <v>0.27</v>
       </c>
       <c r="F1112" t="n">
-        <v>0.24</v>
+        <v>0.275</v>
       </c>
       <c r="G1112" t="n">
-        <v>0.225</v>
+        <v>0.255</v>
       </c>
       <c r="H1112" t="n">
-        <v>0.235</v>
+        <v>0.26</v>
       </c>
       <c r="I1112" t="n">
-        <v>2994800</v>
+        <v>6133400</v>
       </c>
     </row>
     <row r="1113">
       <c r="A1113" t="n">
-        <v>1580256000</v>
+        <v>1579046400</v>
       </c>
       <c r="B1113" t="inlineStr">
         <is>
-          <t>2020-01-29</t>
+          <t>2020-01-15</t>
         </is>
       </c>
       <c r="C1113" t="inlineStr">
@@ -39406,28 +39406,28 @@
         </is>
       </c>
       <c r="E1113" t="n">
-        <v>0.235</v>
+        <v>0.26</v>
       </c>
       <c r="F1113" t="n">
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
       <c r="G1113" t="n">
-        <v>0.235</v>
+        <v>0.25</v>
       </c>
       <c r="H1113" t="n">
-        <v>0.24</v>
+        <v>0.255</v>
       </c>
       <c r="I1113" t="n">
-        <v>2175900</v>
+        <v>2192000</v>
       </c>
     </row>
     <row r="1114">
       <c r="A1114" t="n">
-        <v>1580342400</v>
+        <v>1579132800</v>
       </c>
       <c r="B1114" t="inlineStr">
         <is>
-          <t>2020-01-30</t>
+          <t>2020-01-16</t>
         </is>
       </c>
       <c r="C1114" t="inlineStr">
@@ -39441,28 +39441,28 @@
         </is>
       </c>
       <c r="E1114" t="n">
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
       <c r="F1114" t="n">
-        <v>0.24</v>
+        <v>0.265</v>
       </c>
       <c r="G1114" t="n">
-        <v>0.215</v>
+        <v>0.25</v>
       </c>
       <c r="H1114" t="n">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="I1114" t="n">
-        <v>5183000</v>
+        <v>7498700</v>
       </c>
     </row>
     <row r="1115">
       <c r="A1115" t="n">
-        <v>1580428800</v>
+        <v>1579219200</v>
       </c>
       <c r="B1115" t="inlineStr">
         <is>
-          <t>2020-01-31</t>
+          <t>2020-01-17</t>
         </is>
       </c>
       <c r="C1115" t="inlineStr">
@@ -39476,28 +39476,28 @@
         </is>
       </c>
       <c r="E1115" t="n">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="F1115" t="n">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="G1115" t="n">
-        <v>0.185</v>
+        <v>0.24</v>
       </c>
       <c r="H1115" t="n">
-        <v>0.185</v>
+        <v>0.245</v>
       </c>
       <c r="I1115" t="n">
-        <v>7335800</v>
+        <v>2703700</v>
       </c>
     </row>
     <row r="1116">
       <c r="A1116" t="n">
-        <v>1580688000</v>
+        <v>1579478400</v>
       </c>
       <c r="B1116" t="inlineStr">
         <is>
-          <t>2020-02-03</t>
+          <t>2020-01-20</t>
         </is>
       </c>
       <c r="C1116" t="inlineStr">
@@ -39511,28 +39511,28 @@
         </is>
       </c>
       <c r="E1116" t="n">
-        <v>0.175</v>
+        <v>0.245</v>
       </c>
       <c r="F1116" t="n">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="G1116" t="n">
-        <v>0.175</v>
+        <v>0.24</v>
       </c>
       <c r="H1116" t="n">
-        <v>0.2</v>
+        <v>0.255</v>
       </c>
       <c r="I1116" t="n">
-        <v>3677200</v>
+        <v>4433500</v>
       </c>
     </row>
     <row r="1117">
       <c r="A1117" t="n">
-        <v>1580774400</v>
+        <v>1579564800</v>
       </c>
       <c r="B1117" t="inlineStr">
         <is>
-          <t>2020-02-04</t>
+          <t>2020-01-21</t>
         </is>
       </c>
       <c r="C1117" t="inlineStr">
@@ -39546,28 +39546,28 @@
         </is>
       </c>
       <c r="E1117" t="n">
-        <v>0.205</v>
+        <v>0.26</v>
       </c>
       <c r="F1117" t="n">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="G1117" t="n">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="H1117" t="n">
-        <v>0.22</v>
+        <v>0.245</v>
       </c>
       <c r="I1117" t="n">
-        <v>4327900</v>
+        <v>3318600</v>
       </c>
     </row>
     <row r="1118">
       <c r="A1118" t="n">
-        <v>1580860800</v>
+        <v>1579651200</v>
       </c>
       <c r="B1118" t="inlineStr">
         <is>
-          <t>2020-02-05</t>
+          <t>2020-01-22</t>
         </is>
       </c>
       <c r="C1118" t="inlineStr">
@@ -39581,28 +39581,28 @@
         </is>
       </c>
       <c r="E1118" t="n">
-        <v>0.225</v>
+        <v>0.24</v>
       </c>
       <c r="F1118" t="n">
-        <v>0.225</v>
+        <v>0.245</v>
       </c>
       <c r="G1118" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="H1118" t="n">
-        <v>0.215</v>
+        <v>0.24</v>
       </c>
       <c r="I1118" t="n">
-        <v>2011300</v>
+        <v>2870300</v>
       </c>
     </row>
     <row r="1119">
       <c r="A1119" t="n">
-        <v>1580947200</v>
+        <v>1579737600</v>
       </c>
       <c r="B1119" t="inlineStr">
         <is>
-          <t>2020-02-06</t>
+          <t>2020-01-23</t>
         </is>
       </c>
       <c r="C1119" t="inlineStr">
@@ -39616,28 +39616,28 @@
         </is>
       </c>
       <c r="E1119" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="F1119" t="n">
-        <v>0.235</v>
+        <v>0.255</v>
       </c>
       <c r="G1119" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="H1119" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="I1119" t="n">
-        <v>2867100</v>
+        <v>5798100</v>
       </c>
     </row>
     <row r="1120">
       <c r="A1120" t="n">
-        <v>1581033600</v>
+        <v>1579824000</v>
       </c>
       <c r="B1120" t="inlineStr">
         <is>
-          <t>2020-02-07</t>
+          <t>2020-01-24</t>
         </is>
       </c>
       <c r="C1120" t="inlineStr">
@@ -39651,28 +39651,28 @@
         </is>
       </c>
       <c r="E1120" t="n">
-        <v>0.23</v>
+        <v>0.235</v>
       </c>
       <c r="F1120" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="G1120" t="n">
         <v>0.235</v>
       </c>
-      <c r="G1120" t="n">
-        <v>0.215</v>
-      </c>
       <c r="H1120" t="n">
-        <v>0.215</v>
+        <v>0.245</v>
       </c>
       <c r="I1120" t="n">
-        <v>2937500</v>
+        <v>1280400</v>
       </c>
     </row>
     <row r="1121">
       <c r="A1121" t="n">
-        <v>1581292800</v>
+        <v>1580169600</v>
       </c>
       <c r="B1121" t="inlineStr">
         <is>
-          <t>2020-02-10</t>
+          <t>2020-01-28</t>
         </is>
       </c>
       <c r="C1121" t="inlineStr">
@@ -39686,28 +39686,28 @@
         </is>
       </c>
       <c r="E1121" t="n">
-        <v>0.215</v>
+        <v>0.235</v>
       </c>
       <c r="F1121" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="G1121" t="n">
-        <v>0.205</v>
+        <v>0.225</v>
       </c>
       <c r="H1121" t="n">
-        <v>0.205</v>
+        <v>0.235</v>
       </c>
       <c r="I1121" t="n">
-        <v>2651700</v>
+        <v>2994800</v>
       </c>
     </row>
     <row r="1122">
       <c r="A1122" t="n">
-        <v>1581379200</v>
+        <v>1580256000</v>
       </c>
       <c r="B1122" t="inlineStr">
         <is>
-          <t>2020-02-11</t>
+          <t>2020-01-29</t>
         </is>
       </c>
       <c r="C1122" t="inlineStr">
@@ -39721,28 +39721,28 @@
         </is>
       </c>
       <c r="E1122" t="n">
-        <v>0.21</v>
+        <v>0.235</v>
       </c>
       <c r="F1122" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="G1122" t="n">
-        <v>0.21</v>
+        <v>0.235</v>
       </c>
       <c r="H1122" t="n">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="I1122" t="n">
-        <v>5629900</v>
+        <v>2175900</v>
       </c>
     </row>
     <row r="1123">
       <c r="A1123" t="n">
-        <v>1581465600</v>
+        <v>1580342400</v>
       </c>
       <c r="B1123" t="inlineStr">
         <is>
-          <t>2020-02-12</t>
+          <t>2020-01-30</t>
         </is>
       </c>
       <c r="C1123" t="inlineStr">
@@ -39756,28 +39756,28 @@
         </is>
       </c>
       <c r="E1123" t="n">
-        <v>0.225</v>
+        <v>0.24</v>
       </c>
       <c r="F1123" t="n">
-        <v>0.225</v>
+        <v>0.24</v>
       </c>
       <c r="G1123" t="n">
-        <v>0.21</v>
+        <v>0.215</v>
       </c>
       <c r="H1123" t="n">
-        <v>0.215</v>
+        <v>0.22</v>
       </c>
       <c r="I1123" t="n">
-        <v>3099700</v>
+        <v>5183000</v>
       </c>
     </row>
     <row r="1124">
       <c r="A1124" t="n">
-        <v>1581552000</v>
+        <v>1580428800</v>
       </c>
       <c r="B1124" t="inlineStr">
         <is>
-          <t>2020-02-13</t>
+          <t>2020-01-31</t>
         </is>
       </c>
       <c r="C1124" t="inlineStr">
@@ -39791,28 +39791,28 @@
         </is>
       </c>
       <c r="E1124" t="n">
-        <v>0.215</v>
+        <v>0.22</v>
       </c>
       <c r="F1124" t="n">
-        <v>0.225</v>
+        <v>0.22</v>
       </c>
       <c r="G1124" t="n">
-        <v>0.21</v>
+        <v>0.185</v>
       </c>
       <c r="H1124" t="n">
-        <v>0.22</v>
+        <v>0.185</v>
       </c>
       <c r="I1124" t="n">
-        <v>2752800</v>
+        <v>7335800</v>
       </c>
     </row>
     <row r="1125">
       <c r="A1125" t="n">
-        <v>1581638400</v>
+        <v>1580688000</v>
       </c>
       <c r="B1125" t="inlineStr">
         <is>
-          <t>2020-02-14</t>
+          <t>2020-02-03</t>
         </is>
       </c>
       <c r="C1125" t="inlineStr">
@@ -39826,28 +39826,28 @@
         </is>
       </c>
       <c r="E1125" t="n">
-        <v>0.22</v>
+        <v>0.175</v>
       </c>
       <c r="F1125" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="G1125" t="n">
-        <v>0.21</v>
+        <v>0.175</v>
       </c>
       <c r="H1125" t="n">
-        <v>0.215</v>
+        <v>0.2</v>
       </c>
       <c r="I1125" t="n">
-        <v>1373800</v>
+        <v>3677200</v>
       </c>
     </row>
     <row r="1126">
       <c r="A1126" t="n">
-        <v>1581897600</v>
+        <v>1580774400</v>
       </c>
       <c r="B1126" t="inlineStr">
         <is>
-          <t>2020-02-17</t>
+          <t>2020-02-04</t>
         </is>
       </c>
       <c r="C1126" t="inlineStr">
@@ -39861,7 +39861,7 @@
         </is>
       </c>
       <c r="E1126" t="n">
-        <v>0.21</v>
+        <v>0.205</v>
       </c>
       <c r="F1126" t="n">
         <v>0.22</v>
@@ -39870,19 +39870,19 @@
         <v>0.2</v>
       </c>
       <c r="H1126" t="n">
-        <v>0.205</v>
+        <v>0.22</v>
       </c>
       <c r="I1126" t="n">
-        <v>2701600</v>
+        <v>4327900</v>
       </c>
     </row>
     <row r="1127">
       <c r="A1127" t="n">
-        <v>1581984000</v>
+        <v>1580860800</v>
       </c>
       <c r="B1127" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>2020-02-05</t>
         </is>
       </c>
       <c r="C1127" t="inlineStr">
@@ -39896,28 +39896,28 @@
         </is>
       </c>
       <c r="E1127" t="n">
-        <v>0.205</v>
+        <v>0.225</v>
       </c>
       <c r="F1127" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="G1127" t="n">
         <v>0.21</v>
       </c>
-      <c r="G1127" t="n">
-        <v>0.19</v>
-      </c>
       <c r="H1127" t="n">
-        <v>0.195</v>
+        <v>0.215</v>
       </c>
       <c r="I1127" t="n">
-        <v>3421100</v>
+        <v>2011300</v>
       </c>
     </row>
     <row r="1128">
       <c r="A1128" t="n">
-        <v>1582070400</v>
+        <v>1580947200</v>
       </c>
       <c r="B1128" t="inlineStr">
         <is>
-          <t>2020-02-19</t>
+          <t>2020-02-06</t>
         </is>
       </c>
       <c r="C1128" t="inlineStr">
@@ -39931,28 +39931,28 @@
         </is>
       </c>
       <c r="E1128" t="n">
-        <v>0.195</v>
+        <v>0.22</v>
       </c>
       <c r="F1128" t="n">
-        <v>0.205</v>
+        <v>0.235</v>
       </c>
       <c r="G1128" t="n">
-        <v>0.195</v>
+        <v>0.21</v>
       </c>
       <c r="H1128" t="n">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="I1128" t="n">
-        <v>2260800</v>
+        <v>2867100</v>
       </c>
     </row>
     <row r="1129">
       <c r="A1129" t="n">
-        <v>1582156800</v>
+        <v>1581033600</v>
       </c>
       <c r="B1129" t="inlineStr">
         <is>
-          <t>2020-02-20</t>
+          <t>2020-02-07</t>
         </is>
       </c>
       <c r="C1129" t="inlineStr">
@@ -39966,28 +39966,28 @@
         </is>
       </c>
       <c r="E1129" t="n">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="F1129" t="n">
-        <v>0.21</v>
+        <v>0.235</v>
       </c>
       <c r="G1129" t="n">
-        <v>0.2</v>
+        <v>0.215</v>
       </c>
       <c r="H1129" t="n">
-        <v>0.205</v>
+        <v>0.215</v>
       </c>
       <c r="I1129" t="n">
-        <v>2678700</v>
+        <v>2937500</v>
       </c>
     </row>
     <row r="1130">
       <c r="A1130" t="n">
-        <v>1582243200</v>
+        <v>1581292800</v>
       </c>
       <c r="B1130" t="inlineStr">
         <is>
-          <t>2020-02-21</t>
+          <t>2020-02-10</t>
         </is>
       </c>
       <c r="C1130" t="inlineStr">
@@ -40001,28 +40001,28 @@
         </is>
       </c>
       <c r="E1130" t="n">
+        <v>0.215</v>
+      </c>
+      <c r="F1130" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G1130" t="n">
         <v>0.205</v>
       </c>
-      <c r="F1130" t="n">
+      <c r="H1130" t="n">
         <v>0.205</v>
       </c>
-      <c r="G1130" t="n">
-        <v>0.195</v>
-      </c>
-      <c r="H1130" t="n">
-        <v>0.2</v>
-      </c>
       <c r="I1130" t="n">
-        <v>2767000</v>
+        <v>2651700</v>
       </c>
     </row>
     <row r="1131">
       <c r="A1131" t="n">
-        <v>1582502400</v>
+        <v>1581379200</v>
       </c>
       <c r="B1131" t="inlineStr">
         <is>
-          <t>2020-02-24</t>
+          <t>2020-02-11</t>
         </is>
       </c>
       <c r="C1131" t="inlineStr">
@@ -40036,28 +40036,28 @@
         </is>
       </c>
       <c r="E1131" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="F1131" t="n">
-        <v>0.195</v>
+        <v>0.22</v>
       </c>
       <c r="G1131" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="H1131" t="n">
-        <v>0.185</v>
+        <v>0.22</v>
       </c>
       <c r="I1131" t="n">
-        <v>3594600</v>
+        <v>5629900</v>
       </c>
     </row>
     <row r="1132">
       <c r="A1132" t="n">
-        <v>1582588800</v>
+        <v>1581465600</v>
       </c>
       <c r="B1132" t="inlineStr">
         <is>
-          <t>2020-02-25</t>
+          <t>2020-02-12</t>
         </is>
       </c>
       <c r="C1132" t="inlineStr">
@@ -40071,28 +40071,28 @@
         </is>
       </c>
       <c r="E1132" t="n">
-        <v>0.185</v>
+        <v>0.225</v>
       </c>
       <c r="F1132" t="n">
-        <v>0.195</v>
+        <v>0.225</v>
       </c>
       <c r="G1132" t="n">
-        <v>0.185</v>
+        <v>0.21</v>
       </c>
       <c r="H1132" t="n">
-        <v>0.195</v>
+        <v>0.215</v>
       </c>
       <c r="I1132" t="n">
-        <v>2605100</v>
+        <v>3099700</v>
       </c>
     </row>
     <row r="1133">
       <c r="A1133" t="n">
-        <v>1582675200</v>
+        <v>1581552000</v>
       </c>
       <c r="B1133" t="inlineStr">
         <is>
-          <t>2020-02-26</t>
+          <t>2020-02-13</t>
         </is>
       </c>
       <c r="C1133" t="inlineStr">
@@ -40106,28 +40106,28 @@
         </is>
       </c>
       <c r="E1133" t="n">
-        <v>0.195</v>
+        <v>0.215</v>
       </c>
       <c r="F1133" t="n">
-        <v>0.195</v>
+        <v>0.225</v>
       </c>
       <c r="G1133" t="n">
-        <v>0.185</v>
+        <v>0.21</v>
       </c>
       <c r="H1133" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="I1133" t="n">
-        <v>1983100</v>
+        <v>2752800</v>
       </c>
     </row>
     <row r="1134">
       <c r="A1134" t="n">
-        <v>1582761600</v>
+        <v>1581638400</v>
       </c>
       <c r="B1134" t="inlineStr">
         <is>
-          <t>2020-02-27</t>
+          <t>2020-02-14</t>
         </is>
       </c>
       <c r="C1134" t="inlineStr">
@@ -40141,28 +40141,28 @@
         </is>
       </c>
       <c r="E1134" t="n">
-        <v>0.185</v>
+        <v>0.22</v>
       </c>
       <c r="F1134" t="n">
-        <v>0.185</v>
+        <v>0.22</v>
       </c>
       <c r="G1134" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="H1134" t="n">
-        <v>0.18</v>
+        <v>0.215</v>
       </c>
       <c r="I1134" t="n">
-        <v>3227900</v>
+        <v>1373800</v>
       </c>
     </row>
     <row r="1135">
       <c r="A1135" t="n">
-        <v>1582848000</v>
+        <v>1581897600</v>
       </c>
       <c r="B1135" t="inlineStr">
         <is>
-          <t>2020-02-28</t>
+          <t>2020-02-17</t>
         </is>
       </c>
       <c r="C1135" t="inlineStr">
@@ -40176,28 +40176,28 @@
         </is>
       </c>
       <c r="E1135" t="n">
-        <v>0.175</v>
+        <v>0.21</v>
       </c>
       <c r="F1135" t="n">
-        <v>0.175</v>
+        <v>0.22</v>
       </c>
       <c r="G1135" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="H1135" t="n">
-        <v>0.155</v>
+        <v>0.205</v>
       </c>
       <c r="I1135" t="n">
-        <v>7866200</v>
+        <v>2701600</v>
       </c>
     </row>
     <row r="1136">
       <c r="A1136" t="n">
-        <v>1583107200</v>
+        <v>1581984000</v>
       </c>
       <c r="B1136" t="inlineStr">
         <is>
-          <t>2020-03-02</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="C1136" t="inlineStr">
@@ -40211,28 +40211,28 @@
         </is>
       </c>
       <c r="E1136" t="n">
-        <v>0.155</v>
+        <v>0.205</v>
       </c>
       <c r="F1136" t="n">
-        <v>0.165</v>
+        <v>0.21</v>
       </c>
       <c r="G1136" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="H1136" t="n">
-        <v>0.165</v>
+        <v>0.195</v>
       </c>
       <c r="I1136" t="n">
-        <v>2649800</v>
+        <v>3421100</v>
       </c>
     </row>
     <row r="1137">
       <c r="A1137" t="n">
-        <v>1583193600</v>
+        <v>1582070400</v>
       </c>
       <c r="B1137" t="inlineStr">
         <is>
-          <t>2020-03-03</t>
+          <t>2020-02-19</t>
         </is>
       </c>
       <c r="C1137" t="inlineStr">
@@ -40246,28 +40246,28 @@
         </is>
       </c>
       <c r="E1137" t="n">
-        <v>0.17</v>
+        <v>0.195</v>
       </c>
       <c r="F1137" t="n">
-        <v>0.17</v>
+        <v>0.205</v>
       </c>
       <c r="G1137" t="n">
-        <v>0.155</v>
+        <v>0.195</v>
       </c>
       <c r="H1137" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="I1137" t="n">
-        <v>2610000</v>
+        <v>2260800</v>
       </c>
     </row>
     <row r="1138">
       <c r="A1138" t="n">
-        <v>1583280000</v>
+        <v>1582156800</v>
       </c>
       <c r="B1138" t="inlineStr">
         <is>
-          <t>2020-03-04</t>
+          <t>2020-02-20</t>
         </is>
       </c>
       <c r="C1138" t="inlineStr">
@@ -40281,28 +40281,28 @@
         </is>
       </c>
       <c r="E1138" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="F1138" t="n">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="G1138" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="H1138" t="n">
-        <v>0.16</v>
+        <v>0.205</v>
       </c>
       <c r="I1138" t="n">
-        <v>1282500</v>
+        <v>2678700</v>
       </c>
     </row>
     <row r="1139">
       <c r="A1139" t="n">
-        <v>1583366400</v>
+        <v>1582243200</v>
       </c>
       <c r="B1139" t="inlineStr">
         <is>
-          <t>2020-03-05</t>
+          <t>2020-02-21</t>
         </is>
       </c>
       <c r="C1139" t="inlineStr">
@@ -40316,28 +40316,28 @@
         </is>
       </c>
       <c r="E1139" t="n">
-        <v>0.16</v>
+        <v>0.205</v>
       </c>
       <c r="F1139" t="n">
-        <v>0.17</v>
+        <v>0.205</v>
       </c>
       <c r="G1139" t="n">
-        <v>0.155</v>
+        <v>0.195</v>
       </c>
       <c r="H1139" t="n">
-        <v>0.165</v>
+        <v>0.2</v>
       </c>
       <c r="I1139" t="n">
-        <v>3452400</v>
+        <v>2767000</v>
       </c>
     </row>
     <row r="1140">
       <c r="A1140" t="n">
-        <v>1583452800</v>
+        <v>1582502400</v>
       </c>
       <c r="B1140" t="inlineStr">
         <is>
-          <t>2020-03-06</t>
+          <t>2020-02-24</t>
         </is>
       </c>
       <c r="C1140" t="inlineStr">
@@ -40351,28 +40351,28 @@
         </is>
       </c>
       <c r="E1140" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="F1140" t="n">
-        <v>0.165</v>
+        <v>0.195</v>
       </c>
       <c r="G1140" t="n">
-        <v>0.155</v>
+        <v>0.18</v>
       </c>
       <c r="H1140" t="n">
-        <v>0.16</v>
+        <v>0.185</v>
       </c>
       <c r="I1140" t="n">
-        <v>1217800</v>
+        <v>3594600</v>
       </c>
     </row>
     <row r="1141">
       <c r="A1141" t="n">
-        <v>1583712000</v>
+        <v>1582588800</v>
       </c>
       <c r="B1141" t="inlineStr">
         <is>
-          <t>2020-03-09</t>
+          <t>2020-02-25</t>
         </is>
       </c>
       <c r="C1141" t="inlineStr">
@@ -40386,28 +40386,28 @@
         </is>
       </c>
       <c r="E1141" t="n">
-        <v>0.155</v>
+        <v>0.185</v>
       </c>
       <c r="F1141" t="n">
-        <v>0.155</v>
+        <v>0.195</v>
       </c>
       <c r="G1141" t="n">
-        <v>0.135</v>
+        <v>0.185</v>
       </c>
       <c r="H1141" t="n">
-        <v>0.14</v>
+        <v>0.195</v>
       </c>
       <c r="I1141" t="n">
-        <v>4833200</v>
+        <v>2605100</v>
       </c>
     </row>
     <row r="1142">
       <c r="A1142" t="n">
-        <v>1583798400</v>
+        <v>1582675200</v>
       </c>
       <c r="B1142" t="inlineStr">
         <is>
-          <t>2020-03-10</t>
+          <t>2020-02-26</t>
         </is>
       </c>
       <c r="C1142" t="inlineStr">
@@ -40421,28 +40421,28 @@
         </is>
       </c>
       <c r="E1142" t="n">
-        <v>0.135</v>
+        <v>0.195</v>
       </c>
       <c r="F1142" t="n">
-        <v>0.145</v>
+        <v>0.195</v>
       </c>
       <c r="G1142" t="n">
-        <v>0.135</v>
+        <v>0.185</v>
       </c>
       <c r="H1142" t="n">
-        <v>0.14</v>
+        <v>0.19</v>
       </c>
       <c r="I1142" t="n">
-        <v>2928200</v>
+        <v>1983100</v>
       </c>
     </row>
     <row r="1143">
       <c r="A1143" t="n">
-        <v>1583884800</v>
+        <v>1582761600</v>
       </c>
       <c r="B1143" t="inlineStr">
         <is>
-          <t>2020-03-11</t>
+          <t>2020-02-27</t>
         </is>
       </c>
       <c r="C1143" t="inlineStr">
@@ -40456,28 +40456,28 @@
         </is>
       </c>
       <c r="E1143" t="n">
-        <v>0.145</v>
+        <v>0.185</v>
       </c>
       <c r="F1143" t="n">
-        <v>0.145</v>
+        <v>0.185</v>
       </c>
       <c r="G1143" t="n">
-        <v>0.14</v>
+        <v>0.18</v>
       </c>
       <c r="H1143" t="n">
-        <v>0.14</v>
+        <v>0.18</v>
       </c>
       <c r="I1143" t="n">
-        <v>1390800</v>
+        <v>3227900</v>
       </c>
     </row>
     <row r="1144">
       <c r="A1144" t="n">
-        <v>1583971200</v>
+        <v>1582848000</v>
       </c>
       <c r="B1144" t="inlineStr">
         <is>
-          <t>2020-03-12</t>
+          <t>2020-02-28</t>
         </is>
       </c>
       <c r="C1144" t="inlineStr">
@@ -40491,53 +40491,368 @@
         </is>
       </c>
       <c r="E1144" t="n">
-        <v>0.135</v>
+        <v>0.175</v>
       </c>
       <c r="F1144" t="n">
-        <v>0.135</v>
+        <v>0.175</v>
       </c>
       <c r="G1144" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="H1144" t="n">
-        <v>0.13</v>
+        <v>0.155</v>
       </c>
       <c r="I1144" t="n">
-        <v>1853300</v>
+        <v>7866200</v>
       </c>
     </row>
     <row r="1145">
       <c r="A1145" t="n">
+        <v>1583107200</v>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>2020-03-02</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1145" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="F1145" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="G1145" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H1145" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="I1145" t="n">
+        <v>2649800</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="n">
+        <v>1583193600</v>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>2020-03-03</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1146" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1146" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="F1146" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G1146" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="H1146" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I1146" t="n">
+        <v>2610000</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="n">
+        <v>1583280000</v>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>2020-03-04</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1147" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1147" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F1147" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="G1147" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H1147" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I1147" t="n">
+        <v>1282500</v>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="n">
+        <v>1583366400</v>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>2020-03-05</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1148" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1148" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F1148" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G1148" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="H1148" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="I1148" t="n">
+        <v>3452400</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="n">
+        <v>1583452800</v>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>2020-03-06</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1149" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1149" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F1149" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="G1149" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="H1149" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I1149" t="n">
+        <v>1217800</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="n">
+        <v>1583712000</v>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>2020-03-09</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1150" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1150" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="F1150" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="G1150" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="H1150" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I1150" t="n">
+        <v>4833200</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="n">
+        <v>1583798400</v>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>2020-03-10</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1151" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1151" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="F1151" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="G1151" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="H1151" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I1151" t="n">
+        <v>2928200</v>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="n">
+        <v>1583884800</v>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>2020-03-11</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1152" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1152" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="F1152" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="G1152" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="H1152" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I1152" t="n">
+        <v>1390800</v>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="n">
+        <v>1583971200</v>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>2020-03-12</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1153" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1153" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="F1153" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="G1153" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H1153" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I1153" t="n">
+        <v>1853300</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="n">
         <v>1584057600</v>
       </c>
-      <c r="B1145" t="inlineStr">
+      <c r="B1154" t="inlineStr">
         <is>
           <t>2020-03-13</t>
         </is>
       </c>
-      <c r="C1145" t="inlineStr">
-        <is>
-          <t>0178</t>
-        </is>
-      </c>
-      <c r="D1145" t="inlineStr">
-        <is>
-          <t>SEDANIA</t>
-        </is>
-      </c>
-      <c r="E1145" t="n">
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>0178</t>
+        </is>
+      </c>
+      <c r="D1154" t="inlineStr">
+        <is>
+          <t>SEDANIA</t>
+        </is>
+      </c>
+      <c r="E1154" t="n">
         <v>0.125</v>
       </c>
-      <c r="F1145" t="n">
+      <c r="F1154" t="n">
         <v>0.125</v>
       </c>
-      <c r="G1145" t="n">
+      <c r="G1154" t="n">
         <v>0.11</v>
       </c>
-      <c r="H1145" t="n">
+      <c r="H1154" t="n">
         <v>0.115</v>
       </c>
-      <c r="I1145" t="n">
+      <c r="I1154" t="n">
         <v>3282100</v>
       </c>
     </row>

</xml_diff>